<commit_message>
Create dashboard and add student feature
</commit_message>
<xml_diff>
--- a/src/students.xlsx
+++ b/src/students.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>student_id</t>
   </si>
@@ -25,25 +25,16 @@
     <t>major</t>
   </si>
   <si>
-    <t>avatar</t>
-  </si>
-  <si>
-    <t>HE123456</t>
-  </si>
-  <si>
-    <t>elon musk</t>
+    <t>HE838383</t>
+  </si>
+  <si>
+    <t>Viruss</t>
   </si>
   <si>
     <t>AI1908</t>
   </si>
   <si>
     <t>AI</t>
-  </si>
-  <si>
-    <t>HE123457</t>
-  </si>
-  <si>
-    <t>trump</t>
   </si>
 </sst>
 </file>
@@ -313,36 +304,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>